<commit_message>
XLSX changes from BEXUS 24 flight
Correction from previous mistake in data during floating time.
</commit_message>
<xml_diff>
--- a/Real-time analysis/XLSXs/Sample CSV1.xlsx
+++ b/Real-time analysis/XLSXs/Sample CSV1.xlsx
@@ -58,40 +58,16 @@
     <t>SB_Temp</t>
   </si>
   <si>
-    <t>time (s)</t>
-  </si>
-  <si>
-    <r>
-      <t>T_out (</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C)</t>
-    </r>
-  </si>
-  <si>
     <t>CO2_C (%v/v)</t>
   </si>
   <si>
     <t>O3_C (ppm)</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>T_out</t>
   </si>
 </sst>
 </file>
@@ -101,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,15 +211,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -928,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE80"/>
+  <dimension ref="A1:AE102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -945,9 +912,9 @@
     <col min="24" max="24" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="17.25">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -959,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -989,10 +956,10 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
@@ -1012,7 +979,6 @@
         <v>0.48038199999999998</v>
       </c>
       <c r="G2">
-        <f ca="1">RANDBETWEEN(70,80)</f>
         <v>78</v>
       </c>
       <c r="L2">
@@ -1047,8 +1013,7 @@
         <v>-1.2655529999999999</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G5" ca="1" si="0">RANDBETWEEN(70,80)</f>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L3">
         <v>1001</v>
@@ -1082,8 +1047,7 @@
         <v>-3.8705980000000002</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L4">
         <v>1502</v>
@@ -1117,7 +1081,6 @@
         <v>-6.8002849999999997</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="0"/>
         <v>73</v>
       </c>
       <c r="L5">
@@ -1152,8 +1115,7 @@
         <v>-9.6349549999999997</v>
       </c>
       <c r="G6">
-        <f ca="1">RANDBETWEEN(60,70)</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L6">
         <v>2500</v>
@@ -1187,8 +1149,7 @@
         <v>-13.071399</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G9" ca="1" si="1">RANDBETWEEN(60,70)</f>
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="L7">
         <v>3000</v>
@@ -1222,8 +1183,7 @@
         <v>-16.832483</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L8">
         <v>3502</v>
@@ -1257,8 +1217,7 @@
         <v>-20.328312</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L9">
         <v>4003</v>
@@ -1292,8 +1251,7 @@
         <v>-24.037928999999998</v>
       </c>
       <c r="G10">
-        <f ca="1">RANDBETWEEN(40,55)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10">
         <v>4501</v>
@@ -1327,8 +1285,7 @@
         <v>-27.897988999999999</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G13" ca="1" si="2">RANDBETWEEN(40,55)</f>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L11">
         <v>5000</v>
@@ -1362,8 +1319,7 @@
         <v>-32.173749000000001</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="2"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>5503</v>
@@ -1397,8 +1353,7 @@
         <v>-35.950668999999998</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L13">
         <v>6003</v>
@@ -1432,8 +1387,7 @@
         <v>-39.525678999999997</v>
       </c>
       <c r="G14">
-        <f ca="1">RANDBETWEEN(30,45)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L14">
         <v>6502</v>
@@ -1467,8 +1421,7 @@
         <v>-43.025466999999999</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15" ca="1" si="3">RANDBETWEEN(30,45)</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L15">
         <v>7002</v>
@@ -1502,8 +1455,7 @@
         <v>-46.679656999999999</v>
       </c>
       <c r="G16">
-        <f ca="1">RANDBETWEEN(10,25)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L16">
         <v>7500</v>
@@ -1537,8 +1489,7 @@
         <v>-49.126342000000001</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G19" ca="1" si="4">RANDBETWEEN(10,25)</f>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L17">
         <v>8002</v>
@@ -1572,7 +1523,6 @@
         <v>-50.416988000000003</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
       <c r="L18">
@@ -1607,8 +1557,7 @@
         <v>-49.522244999999998</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="4"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L19">
         <v>9002</v>
@@ -1642,8 +1591,7 @@
         <v>-47.055765999999998</v>
       </c>
       <c r="G20">
-        <f ca="1">RANDBETWEEN(2,10)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L20">
         <v>9502</v>
@@ -1677,8 +1625,7 @@
         <v>-46.465868999999998</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G71" ca="1" si="5">RANDBETWEEN(2,10)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L21">
         <v>10001</v>
@@ -1712,8 +1659,7 @@
         <v>-45.705734999999997</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L22">
         <v>10502</v>
@@ -1747,8 +1693,7 @@
         <v>-44.601163</v>
       </c>
       <c r="G23">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L23">
         <v>11000</v>
@@ -1782,8 +1727,7 @@
         <v>-44.236932000000003</v>
       </c>
       <c r="G24">
-        <f ca="1">RANDBETWEEN(2,10)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L24">
         <v>11500</v>
@@ -1817,8 +1761,7 @@
         <v>-45.487988000000001</v>
       </c>
       <c r="G25">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L25">
         <v>12003</v>
@@ -1852,8 +1795,7 @@
         <v>-43.029426000000001</v>
       </c>
       <c r="G26">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L26">
         <v>12502</v>
@@ -1887,8 +1829,7 @@
         <v>-41.323081000000002</v>
       </c>
       <c r="G27">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L27">
         <v>13000</v>
@@ -1922,8 +1863,7 @@
         <v>-42.087175000000002</v>
       </c>
       <c r="G28">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L28">
         <v>13502</v>
@@ -1946,8 +1886,7 @@
         <v>-43.484715000000001</v>
       </c>
       <c r="G29">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L29">
         <v>14001</v>
@@ -1970,7 +1909,6 @@
         <v>-44.537818999999999</v>
       </c>
       <c r="G30">
-        <f t="shared" ca="1" si="5"/>
         <v>6</v>
       </c>
       <c r="L30">
@@ -1994,7 +1932,6 @@
         <v>-43.453043000000001</v>
       </c>
       <c r="G31">
-        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
       <c r="L31">
@@ -2018,8 +1955,7 @@
         <v>-45.404848000000001</v>
       </c>
       <c r="G32">
-        <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L32">
         <v>15500</v>
@@ -2042,8 +1978,7 @@
         <v>-46.964708000000002</v>
       </c>
       <c r="G33">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L33">
         <v>16002</v>
@@ -2066,8 +2001,7 @@
         <v>-47.693171</v>
       </c>
       <c r="G34">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L34">
         <v>16503</v>
@@ -2090,8 +2024,7 @@
         <v>-46.826141999999997</v>
       </c>
       <c r="G35">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L35">
         <v>17003</v>
@@ -2114,8 +2047,7 @@
         <v>-46.521296</v>
       </c>
       <c r="G36">
-        <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L36">
         <v>17504</v>
@@ -2138,8 +2070,7 @@
         <v>-46.517336999999998</v>
       </c>
       <c r="G37">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L37">
         <v>18001</v>
@@ -2162,8 +2093,7 @@
         <v>-47.899040999999997</v>
       </c>
       <c r="G38">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L38">
         <v>18502</v>
@@ -2186,8 +2116,7 @@
         <v>-49.997329999999998</v>
       </c>
       <c r="G39">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L39">
         <v>19000</v>
@@ -2210,8 +2139,7 @@
         <v>-50.773300999999996</v>
       </c>
       <c r="G40">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L40">
         <v>19503</v>
@@ -2234,8 +2162,7 @@
         <v>-49.134259999999998</v>
       </c>
       <c r="G41">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L41">
         <v>20003</v>
@@ -2258,8 +2185,7 @@
         <v>-48.223681999999997</v>
       </c>
       <c r="G42">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L42">
         <v>20502</v>
@@ -2282,8 +2208,7 @@
         <v>-49.530163999999999</v>
       </c>
       <c r="G43">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L43">
         <v>21003</v>
@@ -2306,8 +2231,7 @@
         <v>-49.648935000000002</v>
       </c>
       <c r="G44">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L44">
         <v>21503</v>
@@ -2330,8 +2254,7 @@
         <v>-52.174799999999998</v>
       </c>
       <c r="G45">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L45">
         <v>22006</v>
@@ -2354,8 +2277,7 @@
         <v>-53.037869999999998</v>
       </c>
       <c r="G46">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L46">
         <v>22505</v>
@@ -2378,8 +2300,7 @@
         <v>-52.578620999999998</v>
       </c>
       <c r="G47">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L47">
         <v>23001</v>
@@ -2402,8 +2323,7 @@
         <v>-52.226267</v>
       </c>
       <c r="G48">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L48">
         <v>23502</v>
@@ -2426,8 +2346,7 @@
         <v>-52.285653000000003</v>
       </c>
       <c r="G49">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L49">
         <v>23998</v>
@@ -2450,8 +2369,7 @@
         <v>-54.007834000000003</v>
       </c>
       <c r="G50">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L50">
         <v>24504</v>
@@ -2474,8 +2392,7 @@
         <v>-52.059987999999997</v>
       </c>
       <c r="G51">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L51">
         <v>25006</v>
@@ -2498,8 +2415,7 @@
         <v>-51.272139000000003</v>
       </c>
       <c r="G52">
-        <f ca="1">RANDBETWEEN(2,10)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L52">
         <v>25501</v>
@@ -2516,8 +2432,7 @@
         <v>-55.563735000000001</v>
       </c>
       <c r="G53">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L53">
         <v>26000</v>
@@ -2534,8 +2449,7 @@
         <v>-38.33005</v>
       </c>
       <c r="G54">
-        <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L54">
         <v>26499</v>
@@ -2543,460 +2457,817 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55">
-        <v>14660</v>
+        <v>7327</v>
       </c>
       <c r="C55">
-        <v>28.853795000000002</v>
+        <v>22.648638999999999</v>
       </c>
       <c r="E55">
-        <v>-59.134785000000001</v>
+        <v>-27.989046999999999</v>
       </c>
       <c r="G55">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L55">
-        <v>25007</v>
+        <v>26476</v>
       </c>
     </row>
     <row r="56" spans="1:16">
       <c r="A56">
-        <v>14661</v>
+        <v>7632</v>
       </c>
       <c r="C56">
-        <v>28.188956999999998</v>
+        <v>22.981058000000001</v>
       </c>
       <c r="E56">
-        <v>-59.225842999999998</v>
+        <v>-22.620594000000001</v>
       </c>
       <c r="G56">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L56">
-        <v>24965</v>
+        <v>26520</v>
       </c>
     </row>
     <row r="57" spans="1:16">
       <c r="A57">
-        <v>14688</v>
+        <v>7918</v>
       </c>
       <c r="C57">
-        <v>32.436534000000002</v>
+        <v>22.574767999999999</v>
       </c>
       <c r="E57">
-        <v>-61.751708000000001</v>
+        <v>-14.512487999999999</v>
       </c>
       <c r="G57">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L57">
-        <v>24032</v>
+        <v>26484</v>
       </c>
     </row>
     <row r="58" spans="1:16">
       <c r="A58">
-        <v>14715</v>
+        <v>8286</v>
       </c>
       <c r="C58">
-        <v>38.087657999999998</v>
+        <v>22.685575</v>
       </c>
       <c r="E58">
-        <v>-59.586115999999997</v>
+        <v>-15.383476</v>
       </c>
       <c r="G58">
-        <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L58">
-        <v>23027</v>
+        <v>26530</v>
       </c>
     </row>
     <row r="59" spans="1:16">
       <c r="A59">
-        <v>14745</v>
+        <v>8444</v>
       </c>
       <c r="C59">
-        <v>43.332492000000002</v>
+        <v>22.168478</v>
       </c>
       <c r="E59">
-        <v>-59.095194999999997</v>
+        <v>-17.141287999999999</v>
       </c>
       <c r="G59">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L59">
-        <v>22017</v>
+        <v>26509</v>
       </c>
     </row>
     <row r="60" spans="1:16">
       <c r="A60">
-        <v>14776</v>
+        <v>8880</v>
       </c>
       <c r="C60">
-        <v>49.685389999999998</v>
+        <v>21.799123999999999</v>
       </c>
       <c r="E60">
-        <v>-58.600315999999999</v>
+        <v>-20.074933999999999</v>
       </c>
       <c r="G60">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L60">
-        <v>21037</v>
+        <v>26551</v>
       </c>
     </row>
     <row r="61" spans="1:16">
       <c r="A61">
-        <v>14812</v>
+        <v>9206</v>
       </c>
       <c r="C61">
-        <v>57.848125000000003</v>
+        <v>22.870252000000001</v>
       </c>
       <c r="E61">
-        <v>-56.050696000000002</v>
+        <v>-23.091719000000001</v>
       </c>
       <c r="G61">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L61">
-        <v>19984</v>
+        <v>26520</v>
       </c>
     </row>
     <row r="62" spans="1:16">
       <c r="A62">
-        <v>14846</v>
+        <v>9526</v>
       </c>
       <c r="C62">
-        <v>66.564892</v>
+        <v>22.537832999999999</v>
       </c>
       <c r="E62">
-        <v>-55.464759000000001</v>
+        <v>-22.687898000000001</v>
       </c>
       <c r="G62">
-        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
       <c r="L62">
-        <v>19080</v>
+        <v>26517</v>
       </c>
     </row>
     <row r="63" spans="1:16">
       <c r="A63">
-        <v>14893</v>
+        <v>9868</v>
       </c>
       <c r="C63">
-        <v>77.571657000000002</v>
+        <v>22.242349000000001</v>
       </c>
       <c r="E63">
-        <v>-53.869267000000001</v>
+        <v>-19.869064000000002</v>
       </c>
       <c r="G63">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L63">
-        <v>18014</v>
+        <v>26531</v>
       </c>
     </row>
     <row r="64" spans="1:16">
       <c r="A64">
-        <v>14942</v>
+        <v>10171</v>
       </c>
       <c r="C64">
-        <v>88.172130999999993</v>
+        <v>22.870252000000001</v>
       </c>
       <c r="E64">
-        <v>-53.006197</v>
+        <v>-16.171323999999998</v>
       </c>
       <c r="G64">
-        <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L64">
-        <v>17018</v>
+        <v>26536</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65">
-        <v>14995</v>
+        <v>10439</v>
       </c>
       <c r="C65">
-        <v>103.500344</v>
+        <v>23.054929000000001</v>
       </c>
       <c r="E65">
-        <v>-50.191322999999997</v>
+        <v>-16.685998999999999</v>
       </c>
       <c r="G65">
-        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
       <c r="L65">
-        <v>16010</v>
+        <v>26489</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66">
-        <v>15049</v>
+        <v>10700</v>
       </c>
       <c r="C66">
-        <v>120.010491</v>
+        <v>23.53509</v>
       </c>
       <c r="E66">
-        <v>-48.552281999999998</v>
+        <v>-13.784025</v>
       </c>
       <c r="G66">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L66">
-        <v>15024</v>
+        <v>26502</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67">
-        <v>15107</v>
+        <v>11066</v>
       </c>
       <c r="C67">
-        <v>137.000799</v>
+        <v>22.685575</v>
       </c>
       <c r="E67">
-        <v>-46.758837999999997</v>
+        <v>-17.869751000000001</v>
       </c>
       <c r="G67">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L67">
-        <v>14067</v>
+        <v>26539</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68">
-        <v>15176</v>
+        <v>11301</v>
       </c>
       <c r="C68">
-        <v>160.491747</v>
+        <v>22.833316</v>
       </c>
       <c r="E68">
-        <v>-46.481706000000003</v>
+        <v>-19.520669000000002</v>
       </c>
       <c r="G68">
-        <f t="shared" ca="1" si="5"/>
         <v>6</v>
       </c>
       <c r="L68">
-        <v>13003</v>
+        <v>26539</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69">
-        <v>15233</v>
+        <v>11803</v>
       </c>
       <c r="C69">
-        <v>180.25221400000001</v>
+        <v>21.688317000000001</v>
       </c>
       <c r="E69">
-        <v>-45.729489000000001</v>
+        <v>-21.717934</v>
       </c>
       <c r="G69">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L69">
-        <v>12209</v>
+        <v>26515</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70">
-        <v>15327</v>
+        <v>12201</v>
       </c>
       <c r="C70">
-        <v>215.45169999999999</v>
+        <v>22.574767999999999</v>
       </c>
       <c r="E70">
-        <v>-45.994743999999997</v>
+        <v>-22.327625000000001</v>
       </c>
       <c r="G70">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L70">
-        <v>11008</v>
+        <v>26483</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="A71">
-        <v>15414</v>
+        <v>12748</v>
       </c>
       <c r="C71">
-        <v>250.06021899999999</v>
+        <v>22.500896999999998</v>
       </c>
       <c r="E71">
-        <v>-47.166618999999997</v>
+        <v>-20.272886</v>
       </c>
       <c r="G71">
-        <f t="shared" ca="1" si="5"/>
         <v>7</v>
       </c>
       <c r="L71">
-        <v>10006</v>
+        <v>26446</v>
       </c>
     </row>
     <row r="72" spans="1:12">
       <c r="A72">
-        <v>15502</v>
+        <v>12999</v>
       </c>
       <c r="C72">
-        <v>292.499053</v>
+        <v>22.907187</v>
       </c>
       <c r="E72">
-        <v>-51.600740000000002</v>
+        <v>-19.631522</v>
       </c>
       <c r="G72">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L72">
-        <v>9001</v>
+        <v>26518</v>
       </c>
     </row>
     <row r="73" spans="1:12">
       <c r="A73">
-        <v>15598</v>
+        <v>13500</v>
       </c>
       <c r="C73">
-        <v>340.44126999999997</v>
+        <v>22.72251</v>
       </c>
       <c r="E73">
-        <v>-49.387638000000003</v>
+        <v>-26.029323999999999</v>
       </c>
       <c r="G73">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="L73">
-        <v>8000</v>
+        <v>26379</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="A74">
-        <v>15695</v>
+        <v>13901</v>
       </c>
       <c r="C74">
-        <v>393.73912799999999</v>
+        <v>23.572025</v>
       </c>
       <c r="E74">
-        <v>-43.654953999999996</v>
+        <v>-33.024940999999998</v>
       </c>
       <c r="G74">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="L74">
-        <v>7018</v>
+        <v>26252</v>
       </c>
     </row>
     <row r="75" spans="1:12">
       <c r="A75">
-        <v>15802</v>
+        <v>14167</v>
       </c>
       <c r="C75">
-        <v>455.97536500000001</v>
+        <v>23.350413</v>
       </c>
       <c r="E75">
-        <v>-37.641177999999996</v>
+        <v>-40.630249999999997</v>
       </c>
       <c r="G75">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="L75">
-        <v>6005</v>
+        <v>26100</v>
       </c>
     </row>
     <row r="76" spans="1:12">
       <c r="A76">
-        <v>15911</v>
+        <v>14417</v>
       </c>
       <c r="C76">
-        <v>520.76014799999996</v>
+        <v>24.753959999999999</v>
       </c>
       <c r="E76">
-        <v>-30.332796999999999</v>
+        <v>-46.026415999999998</v>
       </c>
       <c r="G76">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="L76">
-        <v>5066</v>
+        <v>25908</v>
       </c>
     </row>
     <row r="77" spans="1:12">
       <c r="A77">
-        <v>16041</v>
+        <v>14660</v>
       </c>
       <c r="C77">
-        <v>604.08652900000004</v>
+        <v>28.853795000000002</v>
       </c>
       <c r="E77">
-        <v>-21.717934</v>
+        <v>-59.134785000000001</v>
       </c>
       <c r="G77">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="L77">
-        <v>4002</v>
+        <v>25007</v>
       </c>
     </row>
     <row r="78" spans="1:12">
       <c r="A78">
-        <v>16173</v>
+        <v>14661</v>
       </c>
       <c r="C78">
-        <v>690.03532600000005</v>
+        <v>28.188956999999998</v>
       </c>
       <c r="E78">
-        <v>-14.116584</v>
+        <v>-59.225842999999998</v>
       </c>
       <c r="G78">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="L78">
-        <v>3000</v>
+        <v>24965</v>
       </c>
     </row>
     <row r="79" spans="1:12">
       <c r="A79">
-        <v>16311</v>
+        <v>14688</v>
       </c>
       <c r="C79">
-        <v>784.73782600000004</v>
+        <v>32.436534000000002</v>
       </c>
       <c r="E79">
-        <v>-7.4574850000000001</v>
+        <v>-61.751708000000001</v>
       </c>
       <c r="G79">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="L79">
-        <v>2007</v>
+        <v>24032</v>
       </c>
     </row>
     <row r="80" spans="1:12">
       <c r="A80">
+        <v>14715</v>
+      </c>
+      <c r="C80">
+        <v>38.087657999999998</v>
+      </c>
+      <c r="E80">
+        <v>-59.586115999999997</v>
+      </c>
+      <c r="G80">
+        <v>5</v>
+      </c>
+      <c r="L80">
+        <v>23027</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81">
+        <v>14745</v>
+      </c>
+      <c r="C81">
+        <v>43.332492000000002</v>
+      </c>
+      <c r="E81">
+        <v>-59.095194999999997</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="L81">
+        <v>22017</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82">
+        <v>14776</v>
+      </c>
+      <c r="C82">
+        <v>49.685389999999998</v>
+      </c>
+      <c r="E82">
+        <v>-58.600315999999999</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="L82">
+        <v>21037</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83">
+        <v>14812</v>
+      </c>
+      <c r="C83">
+        <v>57.848125000000003</v>
+      </c>
+      <c r="E83">
+        <v>-56.050696000000002</v>
+      </c>
+      <c r="G83">
+        <v>5</v>
+      </c>
+      <c r="L83">
+        <v>19984</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84">
+        <v>14846</v>
+      </c>
+      <c r="C84">
+        <v>66.564892</v>
+      </c>
+      <c r="E84">
+        <v>-55.464759000000001</v>
+      </c>
+      <c r="G84">
+        <v>3</v>
+      </c>
+      <c r="L84">
+        <v>19080</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85">
+        <v>14893</v>
+      </c>
+      <c r="C85">
+        <v>77.571657000000002</v>
+      </c>
+      <c r="E85">
+        <v>-53.869267000000001</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="L85">
+        <v>18014</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86">
+        <v>14942</v>
+      </c>
+      <c r="C86">
+        <v>88.172130999999993</v>
+      </c>
+      <c r="E86">
+        <v>-53.006197</v>
+      </c>
+      <c r="G86">
+        <v>9</v>
+      </c>
+      <c r="L86">
+        <v>17018</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87">
+        <v>14995</v>
+      </c>
+      <c r="C87">
+        <v>103.500344</v>
+      </c>
+      <c r="E87">
+        <v>-50.191322999999997</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="L87">
+        <v>16010</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88">
+        <v>15049</v>
+      </c>
+      <c r="C88">
+        <v>120.010491</v>
+      </c>
+      <c r="E88">
+        <v>-48.552281999999998</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="L88">
+        <v>15024</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89">
+        <v>15107</v>
+      </c>
+      <c r="C89">
+        <v>137.000799</v>
+      </c>
+      <c r="E89">
+        <v>-46.758837999999997</v>
+      </c>
+      <c r="G89">
+        <v>3</v>
+      </c>
+      <c r="L89">
+        <v>14067</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90">
+        <v>15176</v>
+      </c>
+      <c r="C90">
+        <v>160.491747</v>
+      </c>
+      <c r="E90">
+        <v>-46.481706000000003</v>
+      </c>
+      <c r="G90">
+        <v>6</v>
+      </c>
+      <c r="L90">
+        <v>13003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91">
+        <v>15233</v>
+      </c>
+      <c r="C91">
+        <v>180.25221400000001</v>
+      </c>
+      <c r="E91">
+        <v>-45.729489000000001</v>
+      </c>
+      <c r="G91">
+        <v>6</v>
+      </c>
+      <c r="L91">
+        <v>12209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92">
+        <v>15327</v>
+      </c>
+      <c r="C92">
+        <v>215.45169999999999</v>
+      </c>
+      <c r="E92">
+        <v>-45.994743999999997</v>
+      </c>
+      <c r="G92">
+        <v>10</v>
+      </c>
+      <c r="L92">
+        <v>11008</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93">
+        <v>15414</v>
+      </c>
+      <c r="C93">
+        <v>250.06021899999999</v>
+      </c>
+      <c r="E93">
+        <v>-47.166618999999997</v>
+      </c>
+      <c r="G93">
+        <v>5</v>
+      </c>
+      <c r="L93">
+        <v>10006</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94">
+        <v>15502</v>
+      </c>
+      <c r="C94">
+        <v>292.499053</v>
+      </c>
+      <c r="E94">
+        <v>-51.600740000000002</v>
+      </c>
+      <c r="G94">
+        <v>10</v>
+      </c>
+      <c r="L94">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95">
+        <v>15598</v>
+      </c>
+      <c r="C95">
+        <v>340.44126999999997</v>
+      </c>
+      <c r="E95">
+        <v>-49.387638000000003</v>
+      </c>
+      <c r="G95">
+        <v>15</v>
+      </c>
+      <c r="L95">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96">
+        <v>15695</v>
+      </c>
+      <c r="C96">
+        <v>393.73912799999999</v>
+      </c>
+      <c r="E96">
+        <v>-43.654953999999996</v>
+      </c>
+      <c r="G96">
+        <v>22</v>
+      </c>
+      <c r="L96">
+        <v>7018</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97">
+        <v>15802</v>
+      </c>
+      <c r="C97">
+        <v>455.97536500000001</v>
+      </c>
+      <c r="E97">
+        <v>-37.641177999999996</v>
+      </c>
+      <c r="G97">
+        <v>29</v>
+      </c>
+      <c r="L97">
+        <v>6005</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98">
+        <v>15911</v>
+      </c>
+      <c r="C98">
+        <v>520.76014799999996</v>
+      </c>
+      <c r="E98">
+        <v>-30.332796999999999</v>
+      </c>
+      <c r="G98">
+        <v>35</v>
+      </c>
+      <c r="L98">
+        <v>5066</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99">
+        <v>16041</v>
+      </c>
+      <c r="C99">
+        <v>604.08652900000004</v>
+      </c>
+      <c r="E99">
+        <v>-21.717934</v>
+      </c>
+      <c r="G99">
+        <v>40</v>
+      </c>
+      <c r="L99">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100">
+        <v>16173</v>
+      </c>
+      <c r="C100">
+        <v>690.03532600000005</v>
+      </c>
+      <c r="E100">
+        <v>-14.116584</v>
+      </c>
+      <c r="G100">
+        <v>55</v>
+      </c>
+      <c r="L100">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101">
+        <v>16311</v>
+      </c>
+      <c r="C101">
+        <v>784.73782600000004</v>
+      </c>
+      <c r="E101">
+        <v>-7.4574850000000001</v>
+      </c>
+      <c r="G101">
+        <v>67</v>
+      </c>
+      <c r="L101">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102">
         <v>16443</v>
       </c>
-      <c r="C80">
+      <c r="C102">
         <v>887.30757700000004</v>
       </c>
-      <c r="E80">
+      <c r="E102">
         <v>-2.5284849999999999</v>
       </c>
-      <c r="G80">
+      <c r="G102">
         <v>70</v>
       </c>
-      <c r="L80">
+      <c r="L102">
         <v>1045</v>
       </c>
     </row>

</xml_diff>